<commit_message>
correcao de erros execulta
</commit_message>
<xml_diff>
--- a/mudanca.xlsx
+++ b/mudanca.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$71</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="117">
   <si>
     <t>Serial</t>
   </si>
@@ -45,7 +45,334 @@
     <t>525-890-663</t>
   </si>
   <si>
-    <t>analise</t>
+    <t>526-622-389</t>
+  </si>
+  <si>
+    <t>BOLT_6B</t>
+  </si>
+  <si>
+    <t>527-624-919</t>
+  </si>
+  <si>
+    <t>527-270-212</t>
+  </si>
+  <si>
+    <t>541-361-407</t>
+  </si>
+  <si>
+    <t>541-557-575</t>
+  </si>
+  <si>
+    <t>527-624-879</t>
+  </si>
+  <si>
+    <t>541-360-952</t>
+  </si>
+  <si>
+    <t>525-891-058</t>
+  </si>
+  <si>
+    <t>541-361-068</t>
+  </si>
+  <si>
+    <t>526-518-520</t>
+  </si>
+  <si>
+    <t>541-360-970</t>
+  </si>
+  <si>
+    <t>525-890-909</t>
+  </si>
+  <si>
+    <t>527-270-214</t>
+  </si>
+  <si>
+    <t>525-890-485</t>
+  </si>
+  <si>
+    <t>527-624-135</t>
+  </si>
+  <si>
+    <t>525-890-295</t>
+  </si>
+  <si>
+    <t>525-890-501</t>
+  </si>
+  <si>
+    <t>541-362-278</t>
+  </si>
+  <si>
+    <t>527-624-676</t>
+  </si>
+  <si>
+    <t>6P150454</t>
+  </si>
+  <si>
+    <t>6P150447</t>
+  </si>
+  <si>
+    <t>16195CT32185584</t>
+  </si>
+  <si>
+    <t>BOLT_6E</t>
+  </si>
+  <si>
+    <t>527-270-518</t>
+  </si>
+  <si>
+    <t>526-622-570</t>
+  </si>
+  <si>
+    <t>527-270-373</t>
+  </si>
+  <si>
+    <t>525-891-332</t>
+  </si>
+  <si>
+    <t>BOLT_3A</t>
+  </si>
+  <si>
+    <t>541-362-046</t>
+  </si>
+  <si>
+    <t>526-518-502</t>
+  </si>
+  <si>
+    <t>541-545-007</t>
+  </si>
+  <si>
+    <t>541-362-072</t>
+  </si>
+  <si>
+    <t>527-601-116</t>
+  </si>
+  <si>
+    <t>541-360-940</t>
+  </si>
+  <si>
+    <t>541-361-099</t>
+  </si>
+  <si>
+    <t>541-362-020</t>
+  </si>
+  <si>
+    <t>BOLT_2E</t>
+  </si>
+  <si>
+    <t>541-361-829</t>
+  </si>
+  <si>
+    <t>541-544-559</t>
+  </si>
+  <si>
+    <t>541-362-041</t>
+  </si>
+  <si>
+    <t>541-361-636</t>
+  </si>
+  <si>
+    <t>525-890-620</t>
+  </si>
+  <si>
+    <t>527-601-203</t>
+  </si>
+  <si>
+    <t>541-557-436</t>
+  </si>
+  <si>
+    <t>525-890-420</t>
+  </si>
+  <si>
+    <t>541-374-269</t>
+  </si>
+  <si>
+    <t>541-362-282</t>
+  </si>
+  <si>
+    <t>541-362-048</t>
+  </si>
+  <si>
+    <t>6P149246</t>
+  </si>
+  <si>
+    <t>BOLT_3E</t>
+  </si>
+  <si>
+    <t>541-362-003</t>
+  </si>
+  <si>
+    <t>527-601-110</t>
+  </si>
+  <si>
+    <t>527-270-249</t>
+  </si>
+  <si>
+    <t>527-624-887</t>
+  </si>
+  <si>
+    <t>541-374-162</t>
+  </si>
+  <si>
+    <t>541-360-997</t>
+  </si>
+  <si>
+    <t>BOLT_2G</t>
+  </si>
+  <si>
+    <t>6P149123</t>
+  </si>
+  <si>
+    <t>6P149627</t>
+  </si>
+  <si>
+    <t>527-600-899</t>
+  </si>
+  <si>
+    <t>541-361-205</t>
+  </si>
+  <si>
+    <t>541-373-903</t>
+  </si>
+  <si>
+    <t>527-624-148</t>
+  </si>
+  <si>
+    <t>525-891-236</t>
+  </si>
+  <si>
+    <t>541-557-521</t>
+  </si>
+  <si>
+    <t>541-362-039</t>
+  </si>
+  <si>
+    <t>527-624-526</t>
+  </si>
+  <si>
+    <t>526-622-215</t>
+  </si>
+  <si>
+    <t>527-624-123</t>
+  </si>
+  <si>
+    <t>6P150958</t>
+  </si>
+  <si>
+    <t>541-545-003</t>
+  </si>
+  <si>
+    <t>541-361-001</t>
+  </si>
+  <si>
+    <t>527-624-621</t>
+  </si>
+  <si>
+    <t>541-557-559</t>
+  </si>
+  <si>
+    <t>541-361-486</t>
+  </si>
+  <si>
+    <t>541-373-862</t>
+  </si>
+  <si>
+    <t>6P150630</t>
+  </si>
+  <si>
+    <t>541-544-627</t>
+  </si>
+  <si>
+    <t>527-625-030</t>
+  </si>
+  <si>
+    <t>527-624-578</t>
+  </si>
+  <si>
+    <t>527-600-934</t>
+  </si>
+  <si>
+    <t>541-544-834</t>
+  </si>
+  <si>
+    <t>541-544-593</t>
+  </si>
+  <si>
+    <t>541-557-459</t>
+  </si>
+  <si>
+    <t>541-374-080</t>
+  </si>
+  <si>
+    <t>6P149914</t>
+  </si>
+  <si>
+    <t>541-374-235</t>
+  </si>
+  <si>
+    <t>541-557-489</t>
+  </si>
+  <si>
+    <t>527-624-292</t>
+  </si>
+  <si>
+    <t>541-544-684</t>
+  </si>
+  <si>
+    <t>541-361-149</t>
+  </si>
+  <si>
+    <t>6P149542</t>
+  </si>
+  <si>
+    <t>541-374-282</t>
+  </si>
+  <si>
+    <t>541-361-153</t>
+  </si>
+  <si>
+    <t>541-362-163</t>
+  </si>
+  <si>
+    <t>541-557-253</t>
+  </si>
+  <si>
+    <t>541-361-533</t>
+  </si>
+  <si>
+    <t>541-374-020</t>
+  </si>
+  <si>
+    <t>525-891-239</t>
+  </si>
+  <si>
+    <t>541-361-376</t>
+  </si>
+  <si>
+    <t>1470586215</t>
+  </si>
+  <si>
+    <t>BOLT_1G</t>
+  </si>
+  <si>
+    <t>1470586522</t>
+  </si>
+  <si>
+    <t>1470586464</t>
+  </si>
+  <si>
+    <t>527-600-701</t>
+  </si>
+  <si>
+    <t>541-374-111</t>
+  </si>
+  <si>
+    <t>541-361-317</t>
+  </si>
+  <si>
+    <t>541-373-852</t>
+  </si>
+  <si>
+    <t>541-361-307</t>
   </si>
 </sst>
 </file>
@@ -383,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -405,309 +732,885 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="8" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="8" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="C7"/>
       <c r="D7"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="7">
+        <v>1470586744</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="7">
+        <v>1470586573</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
+      <c r="A29" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
+      <c r="A30" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
+      <c r="A32" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
+      <c r="A33" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
+      <c r="A34" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
+      <c r="A35" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
+      <c r="A36" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
+      <c r="A37" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
+      <c r="A38" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
+      <c r="A41" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6"/>
+      <c r="A42" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="5"/>
-      <c r="B43" s="6"/>
+      <c r="A43" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6"/>
+      <c r="A44" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="5"/>
-      <c r="B45" s="6"/>
+      <c r="A45" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6"/>
+      <c r="A46" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6"/>
+      <c r="A47" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="5"/>
-      <c r="B48" s="6"/>
+      <c r="A48" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="5"/>
-      <c r="B49" s="6"/>
+      <c r="A49" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="5"/>
-      <c r="B50" s="6"/>
+      <c r="A50" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="5"/>
-      <c r="B51" s="6"/>
+      <c r="A51" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="5"/>
-      <c r="B52" s="6"/>
+      <c r="A52" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="5"/>
-      <c r="B53" s="6"/>
+      <c r="A53" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="5"/>
-      <c r="B54" s="6"/>
+      <c r="A54" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="5"/>
-      <c r="B55" s="6"/>
+      <c r="A55" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="5"/>
-      <c r="B56" s="6"/>
+      <c r="A56" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="5"/>
-      <c r="B57" s="6"/>
+      <c r="A57" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="5"/>
-      <c r="B58" s="6"/>
+      <c r="A58" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="5"/>
-      <c r="B59" s="6"/>
+      <c r="A59" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="5"/>
-      <c r="B60" s="6"/>
+      <c r="A60" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="5"/>
-      <c r="B61" s="6"/>
+      <c r="A61" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="5"/>
-      <c r="B62" s="6"/>
+      <c r="A62" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="5"/>
-      <c r="B63" s="6"/>
+      <c r="A63" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="5"/>
-      <c r="B64" s="6"/>
+      <c r="A64" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="5"/>
-      <c r="B65" s="6"/>
+      <c r="A65" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="5"/>
-      <c r="B66" s="6"/>
+      <c r="A66" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="5"/>
-      <c r="B67" s="6"/>
+      <c r="A67" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="5"/>
-      <c r="B68" s="6"/>
+      <c r="A68" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="5"/>
-      <c r="B69" s="6"/>
+      <c r="A69" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="5"/>
-      <c r="B70" s="6"/>
+      <c r="A70" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="5"/>
-      <c r="B71" s="6"/>
+      <c r="A71" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="5"/>
-      <c r="B72" s="6"/>
+      <c r="A72" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B85" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B87" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B89" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B90" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B92" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B93" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B94" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B95" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B97" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B98" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B100" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B101" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B102" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B103" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B104" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B105" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B106" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B107" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B108" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B109" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B110" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>